<commit_message>
Přidání komentářů a úprava kódu.
</commit_message>
<xml_diff>
--- a/question_5.xlsx
+++ b/question_5.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34ae73a913e0631e/!OneKlarka/GitHub/DatovaAkademie_dklarka/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{CBB47126-8F2D-4ABF-B49E-214FB9C309C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA70C666-4BB2-4793-B7FD-E99ACB1389A7}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{CBB47126-8F2D-4ABF-B49E-214FB9C309C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54D6C250-46ED-4939-810D-363210796184}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{DF22F916-6B4B-4349-BE4E-78313C2286C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DF22F916-6B4B-4349-BE4E-78313C2286C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4543,14 +4543,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4816,7 +4816,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{639C2444-AB60-43AF-A3A7-B08075A48758}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{639C2444-AB60-43AF-A3A7-B08075A48758}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="A3:E16" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" showAll="0">
@@ -5902,8 +5902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E83414-D57D-4692-8F5D-CC80B653274C}">
   <dimension ref="A3:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Dodělání READ ME  a pozměnění otázky 5.
</commit_message>
<xml_diff>
--- a/question_5.xlsx
+++ b/question_5.xlsx
@@ -5,24 +5,23 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34ae73a913e0631e/!OneKlarka/GitHub/DatovaAkademie_dklarka/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dklar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{CBB47126-8F2D-4ABF-B49E-214FB9C309C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB6E0918-F38C-4B69-B48E-239B5679D3AE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3379FA3F-D55C-466D-93D2-A8C8EB008634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DF22F916-6B4B-4349-BE4E-78313C2286C5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="graph" sheetId="3" r:id="rId1"/>
     <sheet name="question_5" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">question_5!$A$1:$L$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -214,7 +213,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[question_5.xlsx]Sheet2!PivotTable1</c:name>
+    <c:name>[question_5.xlsx]graph!PivotTable1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -3252,7 +3251,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$3</c:f>
+              <c:f>graph!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3288,7 +3287,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>graph!$A$4:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -3332,7 +3331,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$4:$B$16</c:f>
+              <c:f>graph!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3387,7 +3386,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$C$3</c:f>
+              <c:f>graph!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3423,7 +3422,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>graph!$A$4:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -3467,45 +3466,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$C$4:$C$16</c:f>
+              <c:f>graph!$C$4:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>12.71</c:v>
+                  <c:v>6.77</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.41</c:v>
+                  <c:v>5.57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.1</c:v>
+                  <c:v>2.69</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.34</c:v>
+                  <c:v>-4.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.24</c:v>
+                  <c:v>2.4300000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.96</c:v>
+                  <c:v>1.76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.83</c:v>
+                  <c:v>-0.79</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2200000000000002</c:v>
+                  <c:v>-0.05</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.77</c:v>
+                  <c:v>2.2599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.06</c:v>
+                  <c:v>5.39</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.84</c:v>
+                  <c:v>2.54</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.5299999999999994</c:v>
+                  <c:v>5.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3522,7 +3521,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$3</c:f>
+              <c:f>graph!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3560,7 +3559,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>graph!$A$4:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -3604,7 +3603,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$4:$D$16</c:f>
+              <c:f>graph!$D$4:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3659,7 +3658,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$E$3</c:f>
+              <c:f>graph!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3694,7 +3693,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>graph!$A$4:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -3738,7 +3737,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$E$4:$E$16</c:f>
+              <c:f>graph!$E$4:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4554,7 +4553,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="2" name="graph_5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51957559-2ABB-DB1B-A53B-FF19E57720E2}"/>
@@ -4579,7 +4578,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Klárka Dvořáková" refreshedDate="45649.692159606479" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="12" xr:uid="{EDD26A05-D870-42C8-BF54-8A7C8FCB284F}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Klárka Dvořáková" refreshedDate="45662.68923009259" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="12" xr:uid="{EDD26A05-D870-42C8-BF54-8A7C8FCB284F}">
   <cacheSource type="worksheet">
     <worksheetSource name="question_5"/>
   </cacheSource>
@@ -4625,7 +4624,7 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-4.66" maxValue="5.57"/>
     </cacheField>
     <cacheField name="GDPpct2" numFmtId="4">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-2.34" maxValue="12.71"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-4.66" maxValue="6.77"/>
     </cacheField>
     <cacheField name="wagePct" numFmtId="4">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1.49" maxValue="7.72"/>
@@ -4654,7 +4653,7 @@
     <n v="22537.212500000001"/>
     <n v="21083.724999999999"/>
     <n v="5.57"/>
-    <n v="12.71"/>
+    <n v="6.77"/>
     <n v="6.89"/>
     <n v="6.76"/>
   </r>
@@ -4668,7 +4667,7 @@
     <n v="24272.912499999999"/>
     <n v="22537.212500000001"/>
     <n v="2.69"/>
-    <n v="8.41"/>
+    <n v="5.57"/>
     <n v="7.7"/>
     <n v="6.19"/>
   </r>
@@ -4682,7 +4681,7 @@
     <n v="25022"/>
     <n v="24272.912499999999"/>
     <n v="-4.66"/>
-    <n v="-2.1"/>
+    <n v="2.69"/>
     <n v="3.09"/>
     <n v="-6.41"/>
   </r>
@@ -4696,7 +4695,7 @@
     <n v="25503.575000000001"/>
     <n v="25022"/>
     <n v="2.4300000000000002"/>
-    <n v="-2.34"/>
+    <n v="-4.66"/>
     <n v="1.92"/>
     <n v="1.94"/>
   </r>
@@ -4710,7 +4709,7 @@
     <n v="26100.662499999999"/>
     <n v="25503.575000000001"/>
     <n v="1.76"/>
-    <n v="4.24"/>
+    <n v="2.4300000000000002"/>
     <n v="2.34"/>
     <n v="3.35"/>
   </r>
@@ -4724,7 +4723,7 @@
     <n v="26860.45"/>
     <n v="26100.662499999999"/>
     <n v="-0.79"/>
-    <n v="0.96"/>
+    <n v="1.76"/>
     <n v="2.91"/>
     <n v="6.73"/>
   </r>
@@ -4738,7 +4737,7 @@
     <n v="26460.400000000001"/>
     <n v="26860.45"/>
     <n v="-0.05"/>
-    <n v="-0.83"/>
+    <n v="-0.79"/>
     <n v="-1.49"/>
     <n v="5.0999999999999996"/>
   </r>
@@ -4752,7 +4751,7 @@
     <n v="27145.737499999999"/>
     <n v="26460.400000000001"/>
     <n v="2.2599999999999998"/>
-    <n v="2.2200000000000002"/>
+    <n v="-0.05"/>
     <n v="2.59"/>
     <n v="0.74"/>
   </r>
@@ -4766,7 +4765,7 @@
     <n v="27858.275000000001"/>
     <n v="27145.737499999999"/>
     <n v="5.39"/>
-    <n v="7.77"/>
+    <n v="2.2599999999999998"/>
     <n v="2.62"/>
     <n v="-2.91"/>
   </r>
@@ -4780,7 +4779,7 @@
     <n v="28882.075000000001"/>
     <n v="27858.275000000001"/>
     <n v="2.54"/>
-    <n v="8.06"/>
+    <n v="5.39"/>
     <n v="3.68"/>
     <n v="-1.42"/>
   </r>
@@ -4794,7 +4793,7 @@
     <n v="30671.3"/>
     <n v="28882.075000000001"/>
     <n v="5.17"/>
-    <n v="7.84"/>
+    <n v="2.54"/>
     <n v="6.19"/>
     <n v="10.119999999999999"/>
   </r>
@@ -4808,7 +4807,7 @@
     <n v="33039.025000000001"/>
     <n v="30671.3"/>
     <n v="3.2"/>
-    <n v="8.5299999999999994"/>
+    <n v="5.17"/>
     <n v="7.72"/>
     <n v="2.08"/>
   </r>
@@ -4816,7 +4815,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{639C2444-AB60-43AF-A3A7-B08075A48758}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{639C2444-AB60-43AF-A3A7-B08075A48758}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="A3:E16" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" showAll="0">
@@ -5902,8 +5901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E83414-D57D-4692-8F5D-CC80B653274C}">
   <dimension ref="A3:E16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5945,7 +5944,7 @@
         <v>5.57</v>
       </c>
       <c r="C4" s="1">
-        <v>12.71</v>
+        <v>6.77</v>
       </c>
       <c r="D4" s="1">
         <v>6.89</v>
@@ -5962,7 +5961,7 @@
         <v>2.69</v>
       </c>
       <c r="C5" s="1">
-        <v>8.41</v>
+        <v>5.57</v>
       </c>
       <c r="D5" s="1">
         <v>7.7</v>
@@ -5979,7 +5978,7 @@
         <v>-4.66</v>
       </c>
       <c r="C6" s="1">
-        <v>-2.1</v>
+        <v>2.69</v>
       </c>
       <c r="D6" s="1">
         <v>3.09</v>
@@ -5996,7 +5995,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="C7" s="1">
-        <v>-2.34</v>
+        <v>-4.66</v>
       </c>
       <c r="D7" s="1">
         <v>1.92</v>
@@ -6013,7 +6012,7 @@
         <v>1.76</v>
       </c>
       <c r="C8" s="1">
-        <v>4.24</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="D8" s="1">
         <v>2.34</v>
@@ -6030,7 +6029,7 @@
         <v>-0.79</v>
       </c>
       <c r="C9" s="1">
-        <v>0.96</v>
+        <v>1.76</v>
       </c>
       <c r="D9" s="1">
         <v>2.91</v>
@@ -6047,7 +6046,7 @@
         <v>-0.05</v>
       </c>
       <c r="C10" s="1">
-        <v>-0.83</v>
+        <v>-0.79</v>
       </c>
       <c r="D10" s="1">
         <v>-1.49</v>
@@ -6064,7 +6063,7 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="C11" s="1">
-        <v>2.2200000000000002</v>
+        <v>-0.05</v>
       </c>
       <c r="D11" s="1">
         <v>2.59</v>
@@ -6081,7 +6080,7 @@
         <v>5.39</v>
       </c>
       <c r="C12" s="1">
-        <v>7.77</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="D12" s="1">
         <v>2.62</v>
@@ -6098,7 +6097,7 @@
         <v>2.54</v>
       </c>
       <c r="C13" s="1">
-        <v>8.06</v>
+        <v>5.39</v>
       </c>
       <c r="D13" s="1">
         <v>3.68</v>
@@ -6115,7 +6114,7 @@
         <v>5.17</v>
       </c>
       <c r="C14" s="1">
-        <v>7.84</v>
+        <v>2.54</v>
       </c>
       <c r="D14" s="1">
         <v>6.19</v>
@@ -6132,7 +6131,7 @@
         <v>3.2</v>
       </c>
       <c r="C15" s="1">
-        <v>8.5299999999999994</v>
+        <v>5.17</v>
       </c>
       <c r="D15" s="1">
         <v>7.72</v>
@@ -6149,7 +6148,7 @@
         <v>25.509999999999994</v>
       </c>
       <c r="C16" s="1">
-        <v>55.47</v>
+        <v>29.08</v>
       </c>
       <c r="D16" s="1">
         <v>46.160000000000004</v>
@@ -6168,8 +6167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D2E562-8600-444F-A054-9FA804BFE866}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6253,7 +6252,7 @@
         <v>5.57</v>
       </c>
       <c r="J2" s="1">
-        <v>12.71</v>
+        <v>6.77</v>
       </c>
       <c r="K2" s="1">
         <v>6.89</v>
@@ -6291,7 +6290,7 @@
         <v>2.69</v>
       </c>
       <c r="J3" s="1">
-        <v>8.41</v>
+        <v>5.57</v>
       </c>
       <c r="K3" s="1">
         <v>7.7</v>
@@ -6329,7 +6328,7 @@
         <v>-4.66</v>
       </c>
       <c r="J4" s="1">
-        <v>-2.1</v>
+        <v>2.69</v>
       </c>
       <c r="K4" s="1">
         <v>3.09</v>
@@ -6367,7 +6366,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="J5" s="1">
-        <v>-2.34</v>
+        <v>-4.66</v>
       </c>
       <c r="K5" s="1">
         <v>1.92</v>
@@ -6405,7 +6404,7 @@
         <v>1.76</v>
       </c>
       <c r="J6" s="1">
-        <v>4.24</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="K6" s="1">
         <v>2.34</v>
@@ -6443,7 +6442,7 @@
         <v>-0.79</v>
       </c>
       <c r="J7" s="1">
-        <v>0.96</v>
+        <v>1.76</v>
       </c>
       <c r="K7" s="1">
         <v>2.91</v>
@@ -6481,7 +6480,7 @@
         <v>-0.05</v>
       </c>
       <c r="J8" s="1">
-        <v>-0.83</v>
+        <v>-0.79</v>
       </c>
       <c r="K8" s="1">
         <v>-1.49</v>
@@ -6519,7 +6518,7 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="J9" s="1">
-        <v>2.2200000000000002</v>
+        <v>-0.05</v>
       </c>
       <c r="K9" s="1">
         <v>2.59</v>
@@ -6557,7 +6556,7 @@
         <v>5.39</v>
       </c>
       <c r="J10" s="1">
-        <v>7.77</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="K10" s="1">
         <v>2.62</v>
@@ -6595,7 +6594,7 @@
         <v>2.54</v>
       </c>
       <c r="J11" s="1">
-        <v>8.06</v>
+        <v>5.39</v>
       </c>
       <c r="K11" s="1">
         <v>3.68</v>
@@ -6633,7 +6632,7 @@
         <v>5.17</v>
       </c>
       <c r="J12" s="1">
-        <v>7.84</v>
+        <v>2.54</v>
       </c>
       <c r="K12" s="1">
         <v>6.19</v>
@@ -6671,7 +6670,7 @@
         <v>3.2</v>
       </c>
       <c r="J13" s="1">
-        <v>8.5299999999999994</v>
+        <v>5.17</v>
       </c>
       <c r="K13" s="1">
         <v>7.72</v>
@@ -6685,18 +6684,6 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5338AE-FAB0-4736-9C00-E4C2F3228850}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>